<commit_message>
add UITip & bug fix
</commit_message>
<xml_diff>
--- a/Data/MutiLanguage.xlsx
+++ b/Data/MutiLanguage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13160"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -70,6 +70,15 @@
     <t>go_ahead</t>
   </si>
   <si>
+    <t>wrong_character_selected_tip</t>
+  </si>
+  <si>
+    <t>no_character_selected_tip</t>
+  </si>
+  <si>
+    <t>select_character</t>
+  </si>
+  <si>
     <t>简体中文</t>
   </si>
   <si>
@@ -119,6 +128,15 @@
   </si>
   <si>
     <t>出发</t>
+  </si>
+  <si>
+    <t>错误：未知角色</t>
+  </si>
+  <si>
+    <t>请选择一个角色再继续冒险吧！</t>
+  </si>
+  <si>
+    <t>选择角色</t>
   </si>
   <si>
     <t>English</t>
@@ -1317,10 +1335,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6923076923077" defaultRowHeight="16.8" outlineLevelRow="3"/>
@@ -1328,7 +1346,7 @@
     <col min="1" max="16384" width="20.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,61 +1401,79 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:21">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="P2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="Q2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R2" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="S2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1445,55 +1481,55 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="L3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="M3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="O3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="P3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="Q3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="R3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
add team page & NorneStore logic
</commit_message>
<xml_diff>
--- a/Data/MutiLanguage.xlsx
+++ b/Data/MutiLanguage.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -115,6 +115,15 @@
     <t>town_action_init_error</t>
   </si>
   <si>
+    <t>wooden_sword</t>
+  </si>
+  <si>
+    <t>iron_sword</t>
+  </si>
+  <si>
+    <t>magic_sword</t>
+  </si>
+  <si>
     <t>简体中文</t>
   </si>
   <si>
@@ -209,6 +218,15 @@
   </si>
   <si>
     <t>城镇设施初始化失败！</t>
+  </si>
+  <si>
+    <t>木剑</t>
+  </si>
+  <si>
+    <t>铁剑</t>
+  </si>
+  <si>
+    <t>神魔一念</t>
   </si>
   <si>
     <t>English</t>
@@ -1407,10 +1425,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6923076923077" defaultRowHeight="16.8" outlineLevelRow="3"/>
@@ -1418,7 +1436,7 @@
     <col min="1" max="16384" width="20.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:36">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1518,106 +1536,124 @@
       <c r="AG1" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:36">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="R2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="S2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="T2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="U2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="V2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="W2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="X2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Y2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="Z2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AA2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="AB2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="AC2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AD2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AE2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AF2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AG2" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1625,55 +1661,55 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="I3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="M3" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="N3" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="O3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="P3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="Q3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="R3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
Add team bag drag logic
</commit_message>
<xml_diff>
--- a/Data/MutiLanguage.xlsx
+++ b/Data/MutiLanguage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16160"/>
+    <workbookView windowHeight="16760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>ID</t>
   </si>
@@ -124,6 +124,12 @@
     <t>magic_sword</t>
   </si>
   <si>
+    <t>general_error_tip</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
     <t>简体中文</t>
   </si>
   <si>
@@ -227,6 +233,12 @@
   </si>
   <si>
     <t>神魔一念</t>
+  </si>
+  <si>
+    <t>你捉到了一条虫子，把它给我好吗？我会给你奖励，编号是：</t>
+  </si>
+  <si>
+    <t>未知</t>
   </si>
   <si>
     <t>English</t>
@@ -1425,10 +1437,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AJ4"/>
+  <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AM4" sqref="AM4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6923076923077" defaultRowHeight="16.8" outlineLevelRow="3"/>
@@ -1436,7 +1448,7 @@
     <col min="1" max="16384" width="20.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1545,115 +1557,127 @@
       <c r="AJ1" t="s">
         <v>35</v>
       </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:38">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="P2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="R2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="T2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="U2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="V2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="W2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="X2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Z2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AA2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AB2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AC2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AD2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AE2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AF2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AG2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AH2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AI2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AJ2" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1661,55 +1685,55 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="M3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="N3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="O3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="P3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="Q3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="R3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
add store item & item configuration
</commit_message>
<xml_diff>
--- a/Data/MutiLanguage.xlsx
+++ b/Data/MutiLanguage.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>ID</t>
   </si>
@@ -130,6 +130,84 @@
     <t>unknown</t>
   </si>
   <si>
+    <t>fast_shoes</t>
+  </si>
+  <si>
+    <t>stab_shield</t>
+  </si>
+  <si>
+    <t>arm_shield</t>
+  </si>
+  <si>
+    <t>wood_shield</t>
+  </si>
+  <si>
+    <t>long_arch</t>
+  </si>
+  <si>
+    <t>wood_arch</t>
+  </si>
+  <si>
+    <t>zhuge_bow</t>
+  </si>
+  <si>
+    <t>multi_bow</t>
+  </si>
+  <si>
+    <t>hand_bow</t>
+  </si>
+  <si>
+    <t>shadow_charm</t>
+  </si>
+  <si>
+    <t>exchange_charm</t>
+  </si>
+  <si>
+    <t>silent_charm</t>
+  </si>
+  <si>
+    <t>confine_charm</t>
+  </si>
+  <si>
+    <t>thunder_charm</t>
+  </si>
+  <si>
+    <t>king_arrow</t>
+  </si>
+  <si>
+    <t>treasure_bowl</t>
+  </si>
+  <si>
+    <t>shield_token</t>
+  </si>
+  <si>
+    <t>sword_stone</t>
+  </si>
+  <si>
+    <t>energy_potion</t>
+  </si>
+  <si>
+    <t>angry_potion</t>
+  </si>
+  <si>
+    <t>lucky_potion</t>
+  </si>
+  <si>
+    <t>boutique_feather</t>
+  </si>
+  <si>
+    <t>boutique_rice</t>
+  </si>
+  <si>
+    <t>trophy</t>
+  </si>
+  <si>
+    <t>jerky</t>
+  </si>
+  <si>
+    <t>month_card</t>
+  </si>
+  <si>
     <t>简体中文</t>
   </si>
   <si>
@@ -239,6 +317,84 @@
   </si>
   <si>
     <t>未知</t>
+  </si>
+  <si>
+    <t>极速靴</t>
+  </si>
+  <si>
+    <t>刺盾</t>
+  </si>
+  <si>
+    <t>军盾</t>
+  </si>
+  <si>
+    <t>木盾</t>
+  </si>
+  <si>
+    <t>长弓</t>
+  </si>
+  <si>
+    <t>木弓</t>
+  </si>
+  <si>
+    <t>诸葛连弩</t>
+  </si>
+  <si>
+    <t>连射弩</t>
+  </si>
+  <si>
+    <t>手弩</t>
+  </si>
+  <si>
+    <t>幻影符</t>
+  </si>
+  <si>
+    <t>交换符</t>
+  </si>
+  <si>
+    <t>静默符</t>
+  </si>
+  <si>
+    <t>沉默符</t>
+  </si>
+  <si>
+    <t>奔雷符</t>
+  </si>
+  <si>
+    <t>王之箭矢</t>
+  </si>
+  <si>
+    <t>聚宝盆</t>
+  </si>
+  <si>
+    <t>护盾令</t>
+  </si>
+  <si>
+    <t>剑意石</t>
+  </si>
+  <si>
+    <t>精力药水</t>
+  </si>
+  <si>
+    <t>愤怒药水</t>
+  </si>
+  <si>
+    <t>幸运药水</t>
+  </si>
+  <si>
+    <t>精致彩羽</t>
+  </si>
+  <si>
+    <t>精品稻米</t>
+  </si>
+  <si>
+    <t>奖杯</t>
+  </si>
+  <si>
+    <t>风干肉条</t>
+  </si>
+  <si>
+    <t>月卡</t>
   </si>
   <si>
     <t>English</t>
@@ -1437,18 +1593,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:BL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AM4" sqref="AM4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6923076923077" defaultRowHeight="16.8" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="16384" width="20.6923076923077" customWidth="1"/>
+    <col min="1" max="16381" width="20.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:64">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1563,121 +1719,277 @@
       <c r="AL1" t="s">
         <v>37</v>
       </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:64">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="M2" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="N2" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="O2" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="P2" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="Q2" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="R2" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="S2" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="T2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="U2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="V2" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="W2" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="X2" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="Y2" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="Z2" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="AA2" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="AB2" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="AC2" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="AD2" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="AE2" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="AF2" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="AG2" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="AH2" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="AI2" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="AJ2" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="AK2" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="AL2" t="s">
-        <v>74</v>
+        <v>100</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>114</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>115</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>118</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>119</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>121</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>122</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>123</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>124</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>125</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1685,55 +1997,55 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>132</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>134</v>
       </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="L3" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="M3" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="N3" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="O3" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="P3" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="Q3" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="R3" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
battle equip click logic half complete
</commit_message>
<xml_diff>
--- a/Data/MutiLanguage.xlsx
+++ b/Data/MutiLanguage.xlsx
@@ -115,7 +115,7 @@
     <t>town_action_init_error</t>
   </si>
   <si>
-    <t>wooden_sword</t>
+    <t>wood_sword</t>
   </si>
   <si>
     <t>iron_sword</t>
@@ -1595,8 +1595,8 @@
   <sheetPr/>
   <dimension ref="A1:BL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6923076923077" defaultRowHeight="16.8" outlineLevelRow="3"/>

</xml_diff>

<commit_message>
update game page ui
</commit_message>
<xml_diff>
--- a/Data/MutiLanguage.xlsx
+++ b/Data/MutiLanguage.xlsx
@@ -119,10 +119,10 @@
     <t>train_desc</t>
   </si>
   <si>
-    <t>walk_title</t>
-  </si>
-  <si>
-    <t>walk_desc</t>
+    <t>game_title</t>
+  </si>
+  <si>
+    <t>game_desc</t>
   </si>
   <si>
     <t>restaurant_title</t>
@@ -314,10 +314,10 @@
     <t>作为优秀的鸟\n必须有强壮的身体、肌肉和精神</t>
   </si>
   <si>
-    <t>散步</t>
-  </si>
-  <si>
-    <t>放松你的心情\n猜猜会发生什么</t>
+    <t>游戏厅</t>
+  </si>
+  <si>
+    <t>放松你的心情\再来亿把</t>
   </si>
   <si>
     <t>餐馆</t>
@@ -1620,8 +1620,8 @@
   <sheetPr/>
   <dimension ref="A1:BN4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AJ3" sqref="AJ3"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6923076923077" defaultRowHeight="16.8" outlineLevelRow="3"/>

</xml_diff>

<commit_message>
delay uiWindow close logic
</commit_message>
<xml_diff>
--- a/Data/MutiLanguage.xlsx
+++ b/Data/MutiLanguage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760"/>
+    <workbookView windowWidth="19200" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>ID</t>
   </si>
@@ -227,6 +227,18 @@
     <t>month_card</t>
   </si>
   <si>
+    <t>game_no_money_input</t>
+  </si>
+  <si>
+    <t>game_start_no_point</t>
+  </si>
+  <si>
+    <t>accept_character_beyond_limit</t>
+  </si>
+  <si>
+    <t>accept_character_beyond_limit_plural</t>
+  </si>
+  <si>
     <t>简体中文</t>
   </si>
   <si>
@@ -420,6 +432,18 @@
   </si>
   <si>
     <t>月卡</t>
+  </si>
+  <si>
+    <t>投币的钱都没啦</t>
+  </si>
+  <si>
+    <t>开始游戏需要扣除两百积分</t>
+  </si>
+  <si>
+    <t>队伍成员将超过上限,接收失败</t>
+  </si>
+  <si>
+    <t>队伍成员将超过上限，请先优化成员或单个点击领取</t>
   </si>
   <si>
     <t>English</t>
@@ -1618,18 +1642,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BN4"/>
+  <dimension ref="A1:BR4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
+      <selection activeCell="BR4" sqref="BR4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6923076923077" defaultRowHeight="16.8" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="16383" width="20.6923076923077" customWidth="1"/>
+    <col min="1" max="69" width="20.6923076923077" customWidth="1"/>
+    <col min="70" max="70" width="50.3173076923077" customWidth="1"/>
+    <col min="71" max="16383" width="20.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66">
+    <row r="1" spans="1:70">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1828,205 +1854,229 @@
       <c r="BN1" t="s">
         <v>65</v>
       </c>
+      <c r="BO1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:66">
+    <row r="2" spans="1:70">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="M2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="N2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="O2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="P2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="Q2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="R2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="S2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="T2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="U2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="V2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="W2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="X2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="Y2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="Z2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="AA2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="AB2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="AC2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="AD2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="AE2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="AF2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="AG2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="AH2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="AI2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="AJ2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="AK2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="AL2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="AM2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="AN2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="AO2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AP2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="AQ2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="AR2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="AS2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="AT2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AU2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="AV2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="AW2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="AX2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="AY2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="AZ2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="BA2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="BB2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="BC2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="BD2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="BE2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="BF2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="BG2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="BH2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="BI2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="BJ2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="BK2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="BL2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="BM2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="BN2" t="s">
-        <v>130</v>
+        <v>134</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>136</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -2034,55 +2084,55 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="F3" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="G3" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="H3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="I3" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="J3" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="K3" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="L3" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="M3" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="N3" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="O3" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="P3" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="Q3" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="R3" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
update GetDisplayString half part
</commit_message>
<xml_diff>
--- a/Data/MutiLanguage.xlsx
+++ b/Data/MutiLanguage.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="215">
   <si>
     <t>ID</t>
   </si>
@@ -56,7 +56,7 @@
     <t>language</t>
   </si>
   <si>
-    <t>health</t>
+    <t>maxhp</t>
   </si>
   <si>
     <t>dodge</t>
@@ -239,6 +239,84 @@
     <t>accept_character_beyond_limit_plural</t>
   </si>
   <si>
+    <t>place_character_wrong</t>
+  </si>
+  <si>
+    <t>confine_move_failure</t>
+  </si>
+  <si>
+    <t>energy_move_failure</t>
+  </si>
+  <si>
+    <t>wrong_postion_move_failure</t>
+  </si>
+  <si>
+    <t>quit_battle_muti_click</t>
+  </si>
+  <si>
+    <t>game_over</t>
+  </si>
+  <si>
+    <t>over_hungry_tip</t>
+  </si>
+  <si>
+    <t>slient_attack_failure</t>
+  </si>
+  <si>
+    <t>choose_property_tip</t>
+  </si>
+  <si>
+    <t>change_property_error</t>
+  </si>
+  <si>
+    <t>bag_beyond_limit</t>
+  </si>
+  <si>
+    <t>collect</t>
+  </si>
+  <si>
+    <t>neutral_collect</t>
+  </si>
+  <si>
+    <t>collect_done</t>
+  </si>
+  <si>
+    <t>collecting</t>
+  </si>
+  <si>
+    <t>collect_no_money</t>
+  </si>
+  <si>
+    <t>buy_character_no_money</t>
+  </si>
+  <si>
+    <t>buy_character_beyond_limit</t>
+  </si>
+  <si>
+    <t>buy_food_no_money</t>
+  </si>
+  <si>
+    <t>buy_item_no_money</t>
+  </si>
+  <si>
+    <t>normal_collect</t>
+  </si>
+  <si>
+    <t>quick_collect</t>
+  </si>
+  <si>
+    <t>special_collect</t>
+  </si>
+  <si>
+    <t>collect_info_format</t>
+  </si>
+  <si>
+    <t>merge_done</t>
+  </si>
+  <si>
+    <t>merging</t>
+  </si>
+  <si>
     <t>简体中文</t>
   </si>
   <si>
@@ -446,6 +524,84 @@
     <t>队伍成员将超过上限，请先优化成员或单个点击领取</t>
   </si>
   <si>
+    <t>哎，这里不可以</t>
+  </si>
+  <si>
+    <t>禁锢状态，移动失败</t>
+  </si>
+  <si>
+    <t>能量不足，移动失败</t>
+  </si>
+  <si>
+    <t>目标位置不可用，移动失败</t>
+  </si>
+  <si>
+    <t>催催催，只能跑这么快啦！</t>
+  </si>
+  <si>
+    <t>游戏失败</t>
+  </si>
+  <si>
+    <t>你要撑死这个单位嘛,吃不下啦!</t>
+  </si>
+  <si>
+    <t>沉默状态，攻击失败</t>
+  </si>
+  <si>
+    <t>请先选择一项属性</t>
+  </si>
+  <si>
+    <t>加点时没有足够的可分配点数，减点时可分配点数超过最大值，或是属性不能小于0</t>
+  </si>
+  <si>
+    <t>背包将超过上限,接收失败</t>
+  </si>
+  <si>
+    <t>召集</t>
+  </si>
+  <si>
+    <t>自然召集</t>
+  </si>
+  <si>
+    <t>召集完成!</t>
+  </si>
+  <si>
+    <t>召集中</t>
+  </si>
+  <si>
+    <t>天下可没傻鸟跟吃不起饭的走</t>
+  </si>
+  <si>
+    <t>给不起价就别馋人家身子啦</t>
+  </si>
+  <si>
+    <t>队伍成员将超过上限,购买失败</t>
+  </si>
+  <si>
+    <t>小子，来这吃霸王餐吗</t>
+  </si>
+  <si>
+    <t>冷知识：买东西需要花钱呢</t>
+  </si>
+  <si>
+    <t>普通召集</t>
+  </si>
+  <si>
+    <t>快速召集</t>
+  </si>
+  <si>
+    <t>特别召集</t>
+  </si>
+  <si>
+    <t>红：{0}%\\n蓝：{1}%\\n绿：{2}%\\n经典时尚：{3}%\\n等待时间：{4}d\\n</t>
+  </si>
+  <si>
+    <t>合成完毕</t>
+  </si>
+  <si>
+    <t>合成中</t>
+  </si>
+  <si>
     <t>English</t>
   </si>
   <si>
@@ -495,6 +651,27 @@
   </si>
   <si>
     <t>Let's Go</t>
+  </si>
+  <si>
+    <t>Neutral Collect</t>
+  </si>
+  <si>
+    <t>Collect Done!</t>
+  </si>
+  <si>
+    <t>Collecting</t>
+  </si>
+  <si>
+    <t>Normal Collect</t>
+  </si>
+  <si>
+    <t>Special Collect</t>
+  </si>
+  <si>
+    <t>green：{0}%\\nblue：{1}%\\ngreen：{2}%\\nnormal：{3}%\\nwait time：{4}d\\n</t>
+  </si>
+  <si>
+    <t>Merge Done</t>
   </si>
 </sst>
 </file>
@@ -1642,20 +1819,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BR4"/>
+  <dimension ref="A1:CR4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="BR4" sqref="BR4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6923076923077" defaultRowHeight="16.8" outlineLevelRow="3"/>
   <cols>
     <col min="1" max="69" width="20.6923076923077" customWidth="1"/>
     <col min="70" max="70" width="50.3173076923077" customWidth="1"/>
-    <col min="71" max="16383" width="20.6923076923077" customWidth="1"/>
+    <col min="71" max="73" width="20.6923076923077" customWidth="1"/>
+    <col min="74" max="74" width="27.0865384615385" customWidth="1"/>
+    <col min="75" max="16384" width="20.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70">
+    <row r="1" spans="1:96">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1866,273 +2045,459 @@
       <c r="BR1" t="s">
         <v>69</v>
       </c>
+      <c r="BS1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="2" spans="1:70">
+    <row r="2" spans="1:96">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="L2" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="M2" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="N2" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="O2" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="P2" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="Q2" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="R2" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="S2" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
       <c r="T2" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="U2" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="V2" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="W2" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="X2" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="Y2" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="Z2" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="AA2" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="AB2" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="AC2" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="AD2" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="AE2" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="AF2" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="AG2" t="s">
-        <v>101</v>
+        <v>127</v>
       </c>
       <c r="AH2" t="s">
-        <v>102</v>
+        <v>128</v>
       </c>
       <c r="AI2" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="AJ2" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="AK2" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="AL2" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="AM2" t="s">
-        <v>107</v>
+        <v>133</v>
       </c>
       <c r="AN2" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="AO2" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="AP2" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="AQ2" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="AR2" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="AS2" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="AT2" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="AU2" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="AV2" t="s">
-        <v>116</v>
+        <v>142</v>
       </c>
       <c r="AW2" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="AX2" t="s">
-        <v>118</v>
+        <v>144</v>
       </c>
       <c r="AY2" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="AZ2" t="s">
-        <v>120</v>
+        <v>146</v>
       </c>
       <c r="BA2" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="BB2" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="BC2" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
       <c r="BD2" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="BE2" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="BF2" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="BG2" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="BH2" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="BI2" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="BJ2" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="BK2" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="BL2" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="BM2" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="BN2" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="BO2" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="BP2" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="BQ2" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
       <c r="BR2" t="s">
-        <v>138</v>
+        <v>164</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>166</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>167</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>168</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>169</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>170</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>172</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>173</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>174</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>175</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>176</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>177</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>178</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>179</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>180</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>181</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>182</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>183</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>184</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>185</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>186</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>187</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>188</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>189</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:96">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>194</v>
       </c>
       <c r="F3" t="s">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="G3" t="s">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="H3" t="s">
-        <v>145</v>
+        <v>197</v>
       </c>
       <c r="I3" t="s">
-        <v>146</v>
+        <v>198</v>
       </c>
       <c r="J3" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
       <c r="K3" t="s">
-        <v>148</v>
+        <v>200</v>
       </c>
       <c r="L3" t="s">
-        <v>149</v>
+        <v>201</v>
       </c>
       <c r="M3" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="N3" t="s">
-        <v>151</v>
+        <v>203</v>
       </c>
       <c r="O3" t="s">
-        <v>152</v>
+        <v>204</v>
       </c>
       <c r="P3" t="s">
-        <v>153</v>
+        <v>205</v>
       </c>
       <c r="Q3" t="s">
-        <v>154</v>
+        <v>206</v>
       </c>
       <c r="R3" t="s">
-        <v>155</v>
+        <v>207</v>
+      </c>
+      <c r="CD3" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE3" t="s">
+        <v>208</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>209</v>
+      </c>
+      <c r="CG3" t="s">
+        <v>210</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>211</v>
+      </c>
+      <c r="CN3" t="s">
+        <v>212</v>
+      </c>
+      <c r="CO3" t="s">
+        <v>212</v>
+      </c>
+      <c r="CP3" t="s">
+        <v>213</v>
+      </c>
+      <c r="CQ3" t="s">
+        <v>214</v>
+      </c>
+      <c r="CR3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>

<commit_message>
multi language bug fix & feature ui comlete
</commit_message>
<xml_diff>
--- a/Data/MutiLanguage.xlsx
+++ b/Data/MutiLanguage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7440"/>
+    <workbookView windowWidth="13680" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="223">
   <si>
     <t>ID</t>
   </si>
@@ -317,6 +317,18 @@
     <t>merging</t>
   </si>
   <si>
+    <t>enhance_equip_beyond_num</t>
+  </si>
+  <si>
+    <t>enhance_equip_no_money</t>
+  </si>
+  <si>
+    <t>merge_equip_no_money</t>
+  </si>
+  <si>
+    <t>level_up_in_battle</t>
+  </si>
+  <si>
     <t>简体中文</t>
   </si>
   <si>
@@ -600,6 +612,18 @@
   </si>
   <si>
     <t>合成中</t>
+  </si>
+  <si>
+    <t>今天铁匠已经累啦，明天再说吧</t>
+  </si>
+  <si>
+    <t>强化装备可是个体力活，没钱俺可不干</t>
+  </si>
+  <si>
+    <t>合成装备是个时间活，时间就是金钱，朋友</t>
+  </si>
+  <si>
+    <t>在战斗中渡劫升级乃是兵家大忌</t>
   </si>
   <si>
     <t>English</t>
@@ -1819,10 +1843,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:CR4"/>
+  <dimension ref="A1:CV4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="CS1" workbookViewId="0">
+      <selection activeCell="CW9" sqref="CW9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6923076923077" defaultRowHeight="16.8" outlineLevelRow="3"/>
@@ -1834,7 +1858,7 @@
     <col min="75" max="16384" width="20.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96">
+    <row r="1" spans="1:100">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2123,295 +2147,319 @@
       <c r="CR1" t="s">
         <v>95</v>
       </c>
+      <c r="CS1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="2" spans="1:96">
+    <row r="2" spans="1:100">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="J2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="K2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="L2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="M2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="N2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="O2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="P2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="Q2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="R2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="S2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="T2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="U2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="V2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="W2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="X2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="Y2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="Z2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="AA2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="AB2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="AC2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="AD2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="AE2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="AF2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="AG2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AH2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="AI2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="AJ2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AK2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="AL2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="AM2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="AN2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="AO2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="AP2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="AQ2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="AR2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="AS2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="AT2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="AU2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="AV2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="AW2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="AX2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="AY2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="AZ2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="BA2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="BB2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="BC2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="BD2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="BE2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="BF2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="BG2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="BH2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="BI2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="BJ2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="BK2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="BL2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="BM2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="BN2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="BO2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="BP2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="BQ2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="BR2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="BS2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="BT2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="BU2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="BV2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="BW2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="BX2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="BY2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="BZ2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="CA2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="CB2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="CC2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="CD2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="CE2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="CF2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="CG2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="CH2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="CI2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="CJ2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="CK2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="CL2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="CM2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="CN2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="CO2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="CP2" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="CQ2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="CR2" t="s">
-        <v>190</v>
+        <v>194</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>195</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>196</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>197</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:96">
@@ -2419,82 +2467,82 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="E3" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="G3" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="H3" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="I3" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="J3" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="K3" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="L3" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="M3" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="N3" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="O3" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="P3" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="Q3" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="R3" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="CD3" t="s">
         <v>81</v>
       </c>
       <c r="CE3" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="CF3" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="CG3" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="CM3" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="CN3" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="CO3" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="CP3" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="CQ3" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="CR3" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
add select character battle logic
</commit_message>
<xml_diff>
--- a/Data/MutiLanguage.xlsx
+++ b/Data/MutiLanguage.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="228">
   <si>
     <t>ID</t>
   </si>
@@ -332,6 +332,9 @@
     <t>sell_wheat_no_wheat</t>
   </si>
   <si>
+    <t>start_battle_char_num_invalid</t>
+  </si>
+  <si>
     <t>简体中文</t>
   </si>
   <si>
@@ -632,6 +635,9 @@
     <t>地主家都没余粮了，你在卖神魔</t>
   </si>
   <si>
+    <t>你必须选择一到三个角色以进入战斗</t>
+  </si>
+  <si>
     <t>English</t>
   </si>
   <si>
@@ -702,6 +708,9 @@
   </si>
   <si>
     <t>Merge Done</t>
+  </si>
+  <si>
+    <t>You must select between 1 and 3 items to start the battle.</t>
   </si>
 </sst>
 </file>
@@ -1849,10 +1858,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:CW4"/>
+  <dimension ref="A1:CX4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CS1" workbookViewId="0">
-      <selection activeCell="DA22" sqref="DA22"/>
+      <selection activeCell="DB6" sqref="DB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6923076923077" defaultRowHeight="16.8" outlineLevelRow="3"/>
@@ -1864,7 +1873,7 @@
     <col min="75" max="16384" width="20.6923076923077" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101">
+    <row r="1" spans="1:102">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2168,396 +2177,405 @@
       <c r="CW1" t="s">
         <v>100</v>
       </c>
+      <c r="CX1" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="2" spans="1:101">
+    <row r="2" spans="1:102">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="K2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="N2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="O2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="P2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="R2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="S2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="T2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="U2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="V2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="X2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Y2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Z2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AA2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AB2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AC2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AD2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AE2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AF2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AG2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AH2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AI2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AJ2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AK2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AL2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AM2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AN2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AO2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AP2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AQ2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AR2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AS2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AT2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AU2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AV2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AW2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AX2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AY2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AZ2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="BA2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="BB2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="BC2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="BD2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="BE2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="BF2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="BG2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="BH2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="BI2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="BJ2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BK2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="BL2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BM2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="BN2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="BO2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BP2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="BQ2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="BR2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="BS2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BT2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="BU2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="BV2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="BW2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="BX2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="BY2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="BZ2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="CA2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="CB2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="CC2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="CD2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="CE2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CF2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="CG2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="CH2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="CI2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CJ2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="CK2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="CL2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CM2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="CN2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="CO2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="CP2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="CQ2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="CR2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="CS2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="CT2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="CU2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="CV2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="CW2" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:96">
+    <row r="3" spans="1:102">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="I3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="J3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="K3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="L3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="M3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="N3" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="O3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="P3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="Q3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="R3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="CD3" t="s">
         <v>81</v>
       </c>
       <c r="CE3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="CF3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="CG3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="CM3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="CN3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="CO3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="CP3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="CQ3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="CR3" t="s">
         <v>95</v>
+      </c>
+      <c r="CX3" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>